<commit_message>
version for pre, revised bugs on the 5th floor, including load scene
</commit_message>
<xml_diff>
--- a/assets/scene_convert.xlsx
+++ b/assets/scene_convert.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CocosCreatorProjects\Library_test_v0.9.2\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YZ\Desktop\总\Library_test_v1.0.0_yz\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
   <si>
     <t>Event_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -138,83 +138,167 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>sys/nf2f3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sys/nf3f1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sys/nf3f2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sys/nf3f4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sys/nf4f3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sys/nf4f5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sys/nf5f3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sys/nf3f5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sys/nb1elv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>场景切换事件表1(楼层切换)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MG_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MG_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MG_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GM_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GM_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GM_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComputerRoom1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FinalRoom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stroke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SwitchGame</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SwitchGame</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sys/gm2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sys/gm3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sys/gm1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>sys/nf1f2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>sys/nf2f3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sys/nf3f1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sys/nf3f2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sys/nf3f4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sys/nf4f3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sys/nf4f5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sys/nf5f3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sys/nf3f5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sys/nb1elv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>场景切换事件表1(楼层切换)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>F2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -557,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -573,7 +657,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -609,10 +693,10 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3">
         <v>120</v>
@@ -629,16 +713,16 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
         <v>26</v>
       </c>
       <c r="E4">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="F4">
-        <v>210</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -649,7 +733,7 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
@@ -669,16 +753,16 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="E6">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F6">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -689,10 +773,10 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7">
         <v>65</v>
@@ -709,10 +793,10 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8">
         <v>225</v>
@@ -729,10 +813,10 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9">
         <v>70</v>
@@ -749,10 +833,10 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10">
         <v>15</v>
@@ -769,13 +853,13 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F11">
         <v>25</v>
@@ -789,10 +873,10 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12">
         <v>85</v>
@@ -809,10 +893,10 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13">
         <v>35</v>
@@ -829,16 +913,136 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14">
         <v>150</v>
       </c>
       <c r="F14">
         <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18">
+        <v>143</v>
+      </c>
+      <c r="F18">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>